<commit_message>
Updated colors and fonts
</commit_message>
<xml_diff>
--- a/TCMS - External Pentest Checklist.xlsx
+++ b/TCMS - External Pentest Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Templates\Pentest Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nutt\Documents\GitHub\External-Pentest-Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BCF79F-864D-47F0-BE16-2632210B1C51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9E749A-B0B7-4DAE-8D35-5FF25F4D011B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5175" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-8475" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To Do's" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -230,26 +230,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -260,6 +240,14 @@
       <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -277,13 +265,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD80650"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD80650"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +425,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -463,28 +451,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1119,27 +1107,27 @@
   </sheetPr>
   <dimension ref="A1:X1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="53.85546875" style="10" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="10"/>
     <col min="3" max="3" width="29.42578125" style="10" customWidth="1"/>
     <col min="4" max="16384" width="14.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5"/>
@@ -1195,7 +1183,7 @@
       <c r="X2" s="5"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="39" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1225,7 +1213,7 @@
       <c r="X3" s="5"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="39" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1255,7 +1243,7 @@
       <c r="X4" s="5"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="39" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1345,7 +1333,7 @@
       <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -27430,15 +27418,15 @@
   </sheetPr>
   <dimension ref="A1:W942"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="36" style="9" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" style="9" customWidth="1"/>
     <col min="3" max="16384" width="14.42578125" style="9"/>
   </cols>
   <sheetData>
@@ -51006,9 +50994,9 @@
   </sheetPr>
   <dimension ref="A1:E374"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51021,7 +51009,7 @@
     <col min="6" max="16384" width="14.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>8</v>
       </c>
@@ -51204,109 +51192,109 @@
       <c r="D28" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="47"/>
+      <c r="E28" s="40"/>
     </row>
     <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="47"/>
+      <c r="E29" s="40"/>
     </row>
     <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="47"/>
+      <c r="E30" s="40"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="47"/>
+      <c r="E31" s="40"/>
     </row>
     <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="47"/>
+      <c r="E32" s="40"/>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="47"/>
+      <c r="E33" s="40"/>
     </row>
     <row r="34" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D34" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="47"/>
+      <c r="E34" s="40"/>
     </row>
     <row r="35" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D35" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="47"/>
+      <c r="E35" s="40"/>
     </row>
     <row r="36" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="47"/>
+      <c r="E36" s="40"/>
     </row>
     <row r="37" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D37" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="47"/>
+      <c r="E37" s="40"/>
     </row>
     <row r="38" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D38" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="40"/>
     </row>
     <row r="39" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D39" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="47"/>
+      <c r="E39" s="40"/>
     </row>
     <row r="40" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D40" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="47"/>
+      <c r="E40" s="40"/>
     </row>
     <row r="41" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D41" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="47"/>
+      <c r="E41" s="40"/>
     </row>
     <row r="42" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D42" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="47"/>
+      <c r="E42" s="40"/>
     </row>
     <row r="43" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D43" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="47"/>
+      <c r="E43" s="40"/>
     </row>
     <row r="44" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D44" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="47"/>
+      <c r="E44" s="40"/>
     </row>
     <row r="45" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="47"/>
+      <c r="E45" s="40"/>
     </row>
     <row r="46" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D46" s="19" t="s">
@@ -51378,67 +51366,67 @@
       <c r="D57" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="47"/>
+      <c r="E57" s="40"/>
     </row>
     <row r="58" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D58" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="47"/>
+      <c r="E58" s="40"/>
     </row>
     <row r="59" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D59" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="47"/>
+      <c r="E59" s="40"/>
     </row>
     <row r="60" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D60" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="47"/>
+      <c r="E60" s="40"/>
     </row>
     <row r="61" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D61" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E61" s="47"/>
+      <c r="E61" s="40"/>
     </row>
     <row r="62" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D62" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E62" s="47"/>
+      <c r="E62" s="40"/>
     </row>
     <row r="63" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D63" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="47"/>
+      <c r="E63" s="40"/>
     </row>
     <row r="64" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D64" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E64" s="47"/>
+      <c r="E64" s="40"/>
     </row>
     <row r="65" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D65" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E65" s="47"/>
+      <c r="E65" s="40"/>
     </row>
     <row r="66" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D66" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="47"/>
+      <c r="E66" s="40"/>
     </row>
     <row r="67" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D67" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="47"/>
+      <c r="E67" s="40"/>
     </row>
     <row r="68" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D68" s="19" t="s">
@@ -51498,37 +51486,37 @@
       <c r="D77" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E77" s="47"/>
+      <c r="E77" s="40"/>
     </row>
     <row r="78" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D78" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E78" s="47"/>
+      <c r="E78" s="40"/>
     </row>
     <row r="79" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D79" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E79" s="47"/>
+      <c r="E79" s="40"/>
     </row>
     <row r="80" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D80" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E80" s="47"/>
+      <c r="E80" s="40"/>
     </row>
     <row r="81" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D81" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E81" s="47"/>
+      <c r="E81" s="40"/>
     </row>
     <row r="82" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D82" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E82" s="47"/>
+      <c r="E82" s="40"/>
     </row>
     <row r="83" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D83" s="19" t="s">
@@ -51546,37 +51534,37 @@
       <c r="D85" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E85" s="47"/>
+      <c r="E85" s="40"/>
     </row>
     <row r="86" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D86" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E86" s="47"/>
+      <c r="E86" s="40"/>
     </row>
     <row r="87" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D87" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="47"/>
+      <c r="E87" s="40"/>
     </row>
     <row r="88" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D88" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E88" s="47"/>
+      <c r="E88" s="40"/>
     </row>
     <row r="89" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D89" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E89" s="47"/>
+      <c r="E89" s="40"/>
     </row>
     <row r="90" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D90" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E90" s="47"/>
+      <c r="E90" s="40"/>
     </row>
     <row r="91" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D91" s="4"/>
@@ -52751,7 +52739,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7F78DB-83D2-42F5-B9DA-545C4834A040}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -52760,14 +52750,14 @@
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="46" t="s">
         <v>19</v>
       </c>
     </row>
@@ -53009,7 +52999,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6254F7D-5D20-4885-8698-3982F71C084E}">
   <dimension ref="A1:I1754"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -53019,11 +53011,11 @@
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:9" s="15" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="26"/>
@@ -61583,7 +61575,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62660385-7CC3-468F-9622-0B22918359EE}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -61591,11 +61585,11 @@
     <col min="2" max="2" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="46" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="26"/>
@@ -61685,7 +61679,9 @@
   </sheetPr>
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -61731,7 +61727,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="9"/>
       <c r="C2" s="21"/>
@@ -61759,7 +61755,7 @@
       <c r="Y2" s="26"/>
       <c r="Z2" s="26"/>
     </row>
-    <row r="3" spans="1:26" s="27" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="27" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="9"/>
       <c r="C3" s="21"/>
@@ -61793,7 +61789,7 @@
       <c r="Y4" s="26"/>
       <c r="Z4" s="26"/>
     </row>
-    <row r="5" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="27"/>
       <c r="C5" s="25"/>
@@ -61821,7 +61817,7 @@
       <c r="Y5" s="26"/>
       <c r="Z5" s="26"/>
     </row>
-    <row r="6" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="36"/>
       <c r="C6" s="25"/>
@@ -64966,12 +64962,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65153,15 +65146,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F712B955-C8FA-4553-8367-A36F1BEDE981}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DB47A80-56A7-4A79-9BB6-2CB611F04E9A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b189c7c1-5331-4545-a538-44d31693c438"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -65185,17 +65189,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DB47A80-56A7-4A79-9BB6-2CB611F04E9A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F712B955-C8FA-4553-8367-A36F1BEDE981}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b189c7c1-5331-4545-a538-44d31693c438"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>